<commit_message>
repport es and fr
</commit_message>
<xml_diff>
--- a/repport/Applications found on the internet/applications.xlsx
+++ b/repport/Applications found on the internet/applications.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin\Documents\Internship\Applications\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Internship Documents\Internship\SkinApplication\repport\Applications found on the internet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017F449F-E97C-4F76-883A-6AF31DF02EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB6EB7A-3F30-4C0B-9119-3C022C373962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{8AF21527-3A80-490D-AC5B-CAF2DFB0FF4F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8AF21527-3A80-490D-AC5B-CAF2DFB0FF4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -269,6 +269,13 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="6"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -291,13 +298,6 @@
           <bgColor theme="6"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="6"/>
-        </top>
-      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -327,7 +327,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C73111E3-F6BA-46F6-B38F-950AD2E2649D}" name="Tableau1" displayName="Tableau1" ref="A31:E52" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C73111E3-F6BA-46F6-B38F-950AD2E2649D}" name="Tableau1" displayName="Tableau1" ref="A31:E52" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A31:E52" xr:uid="{C73111E3-F6BA-46F6-B38F-950AD2E2649D}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{04F2F139-2E8B-4102-AC4F-FF881D155213}" name="Name"/>
@@ -640,7 +640,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>